<commit_message>
work hard on weekend
</commit_message>
<xml_diff>
--- a/Save_Excel.xlsx
+++ b/Save_Excel.xlsx
@@ -366,13 +366,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:11">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -403,255 +403,75 @@
       <c r="K1" s="1">
         <v>9</v>
       </c>
-      <c r="L1" s="1">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1">
-        <v>18</v>
-      </c>
-      <c r="U1" s="1">
-        <v>19</v>
-      </c>
-      <c r="V1" s="1">
-        <v>20</v>
-      </c>
-      <c r="W1" s="1">
-        <v>21</v>
-      </c>
-      <c r="X1" s="1">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="1">
-        <v>23</v>
-      </c>
-      <c r="Z1" s="1">
-        <v>24</v>
-      </c>
-      <c r="AA1" s="1">
-        <v>25</v>
-      </c>
-      <c r="AB1" s="1">
-        <v>26</v>
-      </c>
-      <c r="AC1" s="1">
-        <v>27</v>
-      </c>
-      <c r="AD1" s="1">
-        <v>28</v>
-      </c>
-      <c r="AE1" s="1">
-        <v>29</v>
-      </c>
     </row>
-    <row r="2" spans="1:31">
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>314312</v>
+        <v>-0.3999999996542806</v>
       </c>
       <c r="C2">
-        <v>472974</v>
+        <v>-0.2999999996926938</v>
       </c>
       <c r="D2">
-        <v>565170</v>
+        <v>-0.199999999731107</v>
       </c>
       <c r="E2">
-        <v>475710</v>
+        <v>-0.09999999976952034</v>
       </c>
       <c r="F2">
-        <v>352488</v>
+        <v>1.920663628141028e-10</v>
       </c>
       <c r="G2">
-        <v>295276</v>
+        <v>0.1000000001536532</v>
       </c>
       <c r="H2">
-        <v>175048</v>
+        <v>0.2000000001152399</v>
       </c>
       <c r="I2">
-        <v>125754</v>
+        <v>0.3000000000768266</v>
       </c>
       <c r="J2">
-        <v>100104</v>
+        <v>0.4000000000384133</v>
       </c>
       <c r="K2">
-        <v>57016</v>
-      </c>
-      <c r="L2">
-        <v>62220</v>
-      </c>
-      <c r="M2">
-        <v>24874</v>
-      </c>
-      <c r="N2">
-        <v>19766</v>
-      </c>
-      <c r="O2">
-        <v>11496</v>
-      </c>
-      <c r="P2">
-        <v>4174</v>
-      </c>
-      <c r="Q2">
-        <v>7650</v>
-      </c>
-      <c r="R2">
-        <v>4804</v>
-      </c>
-      <c r="S2">
-        <v>2264</v>
-      </c>
-      <c r="T2">
-        <v>1118</v>
-      </c>
-      <c r="U2">
-        <v>410</v>
-      </c>
-      <c r="V2">
-        <v>814</v>
-      </c>
-      <c r="W2">
-        <v>384</v>
-      </c>
-      <c r="X2">
-        <v>200</v>
-      </c>
-      <c r="Y2">
-        <v>236</v>
-      </c>
-      <c r="Z2">
-        <v>194</v>
-      </c>
-      <c r="AA2">
-        <v>134</v>
-      </c>
-      <c r="AB2">
-        <v>102</v>
-      </c>
-      <c r="AC2">
-        <v>56</v>
-      </c>
-      <c r="AD2">
-        <v>8</v>
-      </c>
-      <c r="AE2">
-        <v>6</v>
+        <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.01666666666666667</v>
+        <v>1856</v>
       </c>
       <c r="C3">
-        <v>0.03333333333333333</v>
+        <v>1664</v>
       </c>
       <c r="D3">
-        <v>0.05</v>
+        <v>5596</v>
       </c>
       <c r="E3">
-        <v>0.06666666666666667</v>
+        <v>27432</v>
       </c>
       <c r="F3">
-        <v>0.08333333333333333</v>
+        <v>694176</v>
       </c>
       <c r="G3">
-        <v>0.1</v>
+        <v>2338024</v>
       </c>
       <c r="H3">
-        <v>0.1166666666666667</v>
+        <v>5470</v>
       </c>
       <c r="I3">
-        <v>0.1333333333333333</v>
+        <v>468</v>
       </c>
       <c r="J3">
-        <v>0.15</v>
+        <v>54</v>
       </c>
       <c r="K3">
-        <v>0.1666666666666667</v>
-      </c>
-      <c r="L3">
-        <v>0.1833333333333333</v>
-      </c>
-      <c r="M3">
-        <v>0.2</v>
-      </c>
-      <c r="N3">
-        <v>0.2166666666666667</v>
-      </c>
-      <c r="O3">
-        <v>0.2333333333333333</v>
-      </c>
-      <c r="P3">
-        <v>0.25</v>
-      </c>
-      <c r="Q3">
-        <v>0.2666666666666667</v>
-      </c>
-      <c r="R3">
-        <v>0.2833333333333333</v>
-      </c>
-      <c r="S3">
-        <v>0.3</v>
-      </c>
-      <c r="T3">
-        <v>0.3166666666666667</v>
-      </c>
-      <c r="U3">
-        <v>0.3333333333333333</v>
-      </c>
-      <c r="V3">
-        <v>0.35</v>
-      </c>
-      <c r="W3">
-        <v>0.3666666666666666</v>
-      </c>
-      <c r="X3">
-        <v>0.3833333333333333</v>
-      </c>
-      <c r="Y3">
-        <v>0.4</v>
-      </c>
-      <c r="Z3">
-        <v>0.4166666666666667</v>
-      </c>
-      <c r="AA3">
-        <v>0.4333333333333333</v>
-      </c>
-      <c r="AB3">
-        <v>0.45</v>
-      </c>
-      <c r="AC3">
-        <v>0.4666666666666667</v>
-      </c>
-      <c r="AD3">
-        <v>0.4833333333333333</v>
-      </c>
-      <c r="AE3">
-        <v>0.5</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>